<commit_message>
basic randomization of moves
</commit_message>
<xml_diff>
--- a/src/dance-combo-generator/wwwroot/MoveSpreadsheet.xlsx
+++ b/src/dance-combo-generator/wwwroot/MoveSpreadsheet.xlsx
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1517,7 +1517,7 @@
         <v>59</v>
       </c>
       <c r="D53" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E53" s="1">
         <v>3</v>
@@ -1551,7 +1551,7 @@
         <v>59</v>
       </c>
       <c r="D55" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E55" s="5">
         <v>4</v>
@@ -1568,7 +1568,7 @@
         <v>59</v>
       </c>
       <c r="D56" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E56" s="5">
         <v>4</v>

</xml_diff>

<commit_message>
new controller for determining combo by number of beats; initial algorithm; code cleanup
</commit_message>
<xml_diff>
--- a/src/dance-combo-generator/wwwroot/MoveSpreadsheet.xlsx
+++ b/src/dance-combo-generator/wwwroot/MoveSpreadsheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
   <si>
     <t>Down basic</t>
   </si>
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1066,14 +1066,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D27" s="5">
         <v>1</v>
       </c>
@@ -1081,7 +1083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1098,7 +1100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>

</xml_diff>